<commit_message>
Add: Get template scores
</commit_message>
<xml_diff>
--- a/SEP490_API/wwwroot/Templates/template_score.xlsx
+++ b/SEP490_API/wwwroot/Templates/template_score.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\SEP490_BE\SEP490_API\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF7F68F-CE28-4F3E-AD16-EB5B976D4D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D62D5-FE2E-419D-B20A-D16BDC43A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26295" yWindow="960" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Lớp</t>
   </si>
@@ -39,15 +39,9 @@
     <t>2023-2024</t>
   </si>
   <si>
-    <t>Học kì</t>
-  </si>
-  <si>
     <t>Môn học</t>
   </si>
   <si>
-    <t>Toán</t>
-  </si>
-  <si>
     <t>Cột điểm</t>
   </si>
   <si>
@@ -84,7 +78,16 @@
     <t>Học Kỳ I</t>
   </si>
   <si>
-    <t>Cuối kỳ</t>
+    <t>Miệng</t>
+  </si>
+  <si>
+    <t>Lần thứ</t>
+  </si>
+  <si>
+    <t>Ngữ Văn</t>
+  </si>
+  <si>
+    <t>Học kỳ</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,44 +444,44 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -486,39 +489,39 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -526,17 +529,25 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: API get scores
ByClassBySubject,
ByStudentAllSubject,
ByStudentBySubject
</commit_message>
<xml_diff>
--- a/SEP490_API/wwwroot/Templates/template_score.xlsx
+++ b/SEP490_API/wwwroot/Templates/template_score.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\SEP490_BE\SEP490_API\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D62D5-FE2E-419D-B20A-D16BDC43A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1551B1-4097-4AC9-82DE-63573745BE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1125" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Học Kỳ I</t>
   </si>
   <si>
-    <t>Miệng</t>
-  </si>
-  <si>
     <t>Lần thứ</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Học kỳ</t>
+  </si>
+  <si>
+    <t>Cuối kỳ</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -455,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,12 +463,12 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>1</v>

</xml_diff>